<commit_message>
add excel result IDBR
</commit_message>
<xml_diff>
--- a/K-RRT/excel/setting_KRRT.xlsx
+++ b/K-RRT/excel/setting_KRRT.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IDBR\K-RRT\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IDBR\IRDBR\K-RRT\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32EEFDE-894E-4DF4-B7F0-BC8ABA5E4A87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="no_price" sheetId="2" r:id="rId2"/>
-    <sheet name="price" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
-    <sheet name="tl" sheetId="5" r:id="rId5"/>
+    <sheet name="new_setting" sheetId="7" r:id="rId2"/>
+    <sheet name="no_price" sheetId="2" r:id="rId3"/>
+    <sheet name="price" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
+    <sheet name="tl" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="result_noprice" localSheetId="1">no_price!$C$14:$AE$18</definedName>
-    <definedName name="result_noprice_1" localSheetId="1">no_price!$C$20:$AE$25</definedName>
-    <definedName name="result_price" localSheetId="1">no_price!$C$6:$AE$9</definedName>
-    <definedName name="result_price" localSheetId="2">price!$D$5:$AF$8</definedName>
+    <definedName name="result_noprice" localSheetId="2">no_price!$C$14:$AE$18</definedName>
+    <definedName name="result_noprice_1" localSheetId="2">no_price!$C$20:$AE$25</definedName>
+    <definedName name="result_price" localSheetId="2">no_price!$C$6:$AE$9</definedName>
+    <definedName name="result_price" localSheetId="3">price!$D$5:$AF$8</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,8 +36,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="result_noprice" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="result_noprice" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="950" sourceFile="C:\Users\user\Desktop\IDBR\K-RRT\result_noprice.txt" tab="0" comma="1">
       <textFields count="29">
         <textField/>
@@ -70,7 +72,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="result_noprice1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="result_noprice1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="950" sourceFile="C:\Users\user\Desktop\IDBR\K-RRT\result_noprice.txt" tab="0" comma="1">
       <textFields count="29">
         <textField/>
@@ -105,7 +107,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="result_price" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="result_price" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="950" sourceFile="C:\Users\user\Desktop\IDBR\K-RRT\result_price.txt" tab="0" comma="1">
       <textFields count="26">
         <textField/>
@@ -137,7 +139,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="result_price2" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="result_price2" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="950" sourceFile="C:\Users\user\Desktop\IDBR\K-RRT\result_price.txt" tab="0" comma="1">
       <textFields count="26">
         <textField/>
@@ -173,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="48">
   <si>
     <t>AP1</t>
   </si>
@@ -322,7 +324,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -415,19 +417,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="result_noprice_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_price" connectionId="4" xr16:uid="{00000000-0016-0000-0100-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="result_noprice" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_noprice_1" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="result_price" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_noprice" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="result_price" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_price" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,22 +694,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12:N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>5</v>
       </c>
@@ -748,7 +750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -797,7 +799,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -846,7 +848,7 @@
         <v>1.0666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>2</v>
       </c>
@@ -895,7 +897,7 @@
         <v>0.45714285714285713</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -944,7 +946,7 @@
         <v>1.0666666666666667</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -993,7 +995,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>45</v>
       </c>
@@ -1037,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1</v>
       </c>
@@ -1089,7 +1091,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>0.22857142857142856</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>4</v>
       </c>
@@ -1193,7 +1195,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3</v>
       </c>
@@ -1245,7 +1247,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>5</v>
       </c>
@@ -1297,7 +1299,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>47</v>
       </c>
@@ -1346,13 +1348,13 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="M18">
         <f>AVERAGE(M12:M16)</f>
         <v>67.584000000000017</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>8</v>
       </c>
@@ -1378,7 +1380,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>0</v>
       </c>
@@ -1408,7 +1410,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>1</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>48.666666666666664</v>
       </c>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>2</v>
       </c>
@@ -1468,7 +1470,7 @@
         <v>61.833333333333336</v>
       </c>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>3</v>
       </c>
@@ -1498,7 +1500,7 @@
         <v>39.166666666666664</v>
       </c>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>4</v>
       </c>
@@ -1528,7 +1530,7 @@
         <v>59.666666666666664</v>
       </c>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>46</v>
       </c>
@@ -1564,45 +1566,911 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D933FD4B-5259-4884-AA5C-17A8B46C56F1}">
+  <dimension ref="B3:P25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F8" si="0">1/P4</f>
+        <v>0.625</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G8" si="1">E4/F4</f>
+        <v>3.2</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>250</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M8" si="2">L4*J4</f>
+        <v>125</v>
+      </c>
+      <c r="N4">
+        <f>(L4*8)/(H4+I4)</f>
+        <v>200</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <f>(O4*8)/(H4+I4)</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.9375</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>4.2666666666666666</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>0.75</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>250</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>187.5</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N8" si="3">(L5*8)/(H5+I5)</f>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P8" si="4">(O5*8)/(H5+I5)</f>
+        <v>1.0666666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <f>1/P6</f>
+        <v>2.1875</v>
+      </c>
+      <c r="G6">
+        <f>E6/F6</f>
+        <v>4.5714285714285712</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>1.25</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>250</v>
+      </c>
+      <c r="M6">
+        <f>L6*J6</f>
+        <v>312.5</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>57.142857142857146</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>0.45714285714285713</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.9375</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>0.5</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>250</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>133.33333333333334</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>1.0666666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>250</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F13" si="5">1/P12</f>
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G13" si="6">E12/F12</f>
+        <v>0.4</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>60</v>
+      </c>
+      <c r="J12">
+        <v>0.02</v>
+      </c>
+      <c r="K12">
+        <v>500</v>
+      </c>
+      <c r="L12">
+        <v>3072</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12:M13" si="7">L12*J12</f>
+        <v>61.44</v>
+      </c>
+      <c r="N12">
+        <f>(L12*8)/(H12+I12)</f>
+        <v>307.2</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <f>(O12*8)/(H12+I12)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="6"/>
+        <v>0.8</v>
+      </c>
+      <c r="H13">
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <v>60</v>
+      </c>
+      <c r="J13">
+        <v>0.05</v>
+      </c>
+      <c r="K13">
+        <v>500</v>
+      </c>
+      <c r="L13">
+        <v>3072</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="7"/>
+        <v>153.60000000000002</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ref="N13:N17" si="8">(L13*8)/(H13+I13)</f>
+        <v>307.2</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ref="P13:P17" si="9">(O13*8)/(H13+I13)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <f>1/P14</f>
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <f>E14/F14</f>
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>20</v>
+      </c>
+      <c r="I14">
+        <v>60</v>
+      </c>
+      <c r="J14">
+        <v>0.01</v>
+      </c>
+      <c r="K14">
+        <v>500</v>
+      </c>
+      <c r="L14">
+        <v>3072</v>
+      </c>
+      <c r="M14">
+        <f>L14*J14</f>
+        <v>30.72</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="8"/>
+        <v>307.2</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="9"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15:F17" si="10">1/P15</f>
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15:G17" si="11">E15/F15</f>
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <v>60</v>
+      </c>
+      <c r="J15">
+        <v>0.02</v>
+      </c>
+      <c r="K15">
+        <v>500</v>
+      </c>
+      <c r="L15">
+        <v>3072</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15:M17" si="12">L15*J15</f>
+        <v>61.44</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="8"/>
+        <v>307.2</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="9"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+      <c r="I16">
+        <v>60</v>
+      </c>
+      <c r="J16">
+        <v>0.01</v>
+      </c>
+      <c r="K16">
+        <v>500</v>
+      </c>
+      <c r="L16">
+        <v>3072</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="12"/>
+        <v>30.72</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="8"/>
+        <v>307.2</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="9"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+      <c r="I17">
+        <v>60</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>500</v>
+      </c>
+      <c r="L17">
+        <v>3072</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="8"/>
+        <v>307.2</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="9"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f>AVERAGE(M12:M16)</f>
+        <v>67.584000000000017</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>60</v>
+      </c>
+      <c r="E20">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+      <c r="G20">
+        <v>80</v>
+      </c>
+      <c r="H20">
+        <v>30</v>
+      </c>
+      <c r="I20">
+        <v>30</v>
+      </c>
+      <c r="J20">
+        <v>30</v>
+      </c>
+      <c r="K20">
+        <f>((E20*H20)+(F20*I20)+(G20*J20))/(H20+I20+J20)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>60</v>
+      </c>
+      <c r="I21">
+        <v>60</v>
+      </c>
+      <c r="J21">
+        <v>60</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:K25" si="13">((E21*H21)+(F21*I21)+(G21*J21))/(H21+I21+J21)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>60</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>80</v>
+      </c>
+      <c r="G22">
+        <v>90</v>
+      </c>
+      <c r="H22">
+        <v>150</v>
+      </c>
+      <c r="I22">
+        <v>150</v>
+      </c>
+      <c r="J22">
+        <v>150</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="13"/>
+        <v>58.333333333333336</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>60</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+      <c r="G23">
+        <v>120</v>
+      </c>
+      <c r="H23">
+        <v>100</v>
+      </c>
+      <c r="I23">
+        <v>100</v>
+      </c>
+      <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="13"/>
+        <v>58.333333333333336</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>60</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>80</v>
+      </c>
+      <c r="G24">
+        <v>90</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="13"/>
+        <v>58.333333333333336</v>
+      </c>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25">
+        <v>60</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>65</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+      <c r="H25">
+        <v>300</v>
+      </c>
+      <c r="I25">
+        <v>300</v>
+      </c>
+      <c r="J25">
+        <v>300</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="13"/>
+        <v>55.333333333333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C4:AF24"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="7.77734375" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" customWidth="1"/>
-    <col min="5" max="5" width="4.5546875" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="4.33203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" customWidth="1"/>
-    <col min="12" max="12" width="9.21875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.21875" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" customWidth="1"/>
-    <col min="16" max="16" width="9.5546875" customWidth="1"/>
-    <col min="17" max="17" width="7.77734375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="6.44140625" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="7.77734375" customWidth="1"/>
-    <col min="21" max="21" width="6.44140625" customWidth="1"/>
-    <col min="22" max="23" width="7.77734375" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="7.7109375" customWidth="1"/>
+    <col min="21" max="21" width="6.42578125" customWidth="1"/>
+    <col min="22" max="23" width="7.7109375" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" customWidth="1"/>
     <col min="25" max="25" width="11" customWidth="1"/>
-    <col min="26" max="26" width="7.77734375" customWidth="1"/>
-    <col min="27" max="27" width="6.44140625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="7.77734375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="13.77734375" customWidth="1"/>
-    <col min="30" max="30" width="8.6640625" customWidth="1"/>
+    <col min="26" max="26" width="7.7109375" customWidth="1"/>
+    <col min="27" max="27" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="7.7109375" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" customWidth="1"/>
+    <col min="30" max="30" width="8.7109375" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1644,7 +2512,7 @@
       <c r="AE4" s="6"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1736,7 +2604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>100000</v>
       </c>
@@ -1825,7 +2693,7 @@
         <v>1.152547</v>
       </c>
     </row>
-    <row r="7" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>100000</v>
       </c>
@@ -1914,7 +2782,7 @@
         <v>1.066522</v>
       </c>
     </row>
-    <row r="8" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>100000</v>
       </c>
@@ -2003,7 +2871,7 @@
         <v>1.066827</v>
       </c>
     </row>
-    <row r="9" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>100000</v>
       </c>
@@ -2092,7 +2960,7 @@
         <v>1.0686199999999999</v>
       </c>
     </row>
-    <row r="10" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:32" x14ac:dyDescent="0.25">
       <c r="M10">
         <v>7.5</v>
       </c>
@@ -2100,7 +2968,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="13" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:32" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>28</v>
       </c>
@@ -2174,7 +3042,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:32" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>28</v>
       </c>
@@ -2249,7 +3117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:32" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>28</v>
       </c>
@@ -2324,7 +3192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="3:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:32" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>28</v>
       </c>
@@ -2399,42 +3267,42 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="18:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="18:30" x14ac:dyDescent="0.25">
       <c r="R17" s="1"/>
       <c r="U17" s="1"/>
       <c r="X17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="20" spans="18:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="18:30" x14ac:dyDescent="0.25">
       <c r="R20" s="1"/>
       <c r="U20" s="1"/>
       <c r="X20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="18:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="18:30" x14ac:dyDescent="0.25">
       <c r="R21" s="1"/>
       <c r="U21" s="1"/>
       <c r="X21" s="1"/>
       <c r="AA21" s="1"/>
       <c r="AD21" s="1"/>
     </row>
-    <row r="22" spans="18:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="18:30" x14ac:dyDescent="0.25">
       <c r="R22" s="1"/>
       <c r="U22" s="1"/>
       <c r="X22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="18:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="18:30" x14ac:dyDescent="0.25">
       <c r="R23" s="1"/>
       <c r="U23" s="1"/>
       <c r="X23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
-    <row r="24" spans="18:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="18:30" x14ac:dyDescent="0.25">
       <c r="R24" s="1"/>
       <c r="U24" s="1"/>
       <c r="X24" s="1"/>
@@ -2450,52 +3318,51 @@
     <mergeCell ref="AA4:AE4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AD13" r:id="rId1"/>
-    <hyperlink ref="AD14:AD16" r:id="rId2" display="\\"/>
+    <hyperlink ref="AD13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="AD14:AD16" r:id="rId2" display="\\" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:AJ20"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.77734375" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" customWidth="1"/>
-    <col min="13" max="13" width="7.21875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="14" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" customWidth="1"/>
     <col min="16" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.6640625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="9.33203125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="9.109375" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" customWidth="1"/>
     <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="7" hidden="1" customWidth="1"/>
     <col min="25" max="26" width="7" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="6.88671875" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="6.85546875" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="8" customWidth="1"/>
-    <col min="31" max="31" width="8.5546875" customWidth="1"/>
+    <col min="31" max="31" width="8.5703125" customWidth="1"/>
     <col min="32" max="32" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -2537,7 +3404,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="3"/>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
@@ -2629,7 +3496,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>100000</v>
       </c>
@@ -2676,7 +3543,7 @@
         <v>1.152547</v>
       </c>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -2741,7 +3608,7 @@
         <v>1.066522</v>
       </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>100000</v>
       </c>
@@ -2818,7 +3685,7 @@
         <v>1.066827</v>
       </c>
     </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>100000</v>
       </c>
@@ -2895,7 +3762,7 @@
         <v>1.0686199999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>100000</v>
       </c>
@@ -2987,7 +3854,7 @@
         <v>1.0498749999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>30</v>
       </c>
@@ -3049,7 +3916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>30</v>
       </c>
@@ -3117,7 +3984,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="6:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:36" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>30</v>
       </c>
@@ -3200,7 +4067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="6:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:36" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>30</v>
       </c>
@@ -3283,7 +4150,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="6:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:36" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>30</v>
       </c>
@@ -3372,7 +4239,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="6:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:36" x14ac:dyDescent="0.25">
       <c r="AJ20" t="s">
         <v>3</v>
       </c>
@@ -3386,25 +4253,25 @@
     <mergeCell ref="AB3:AF3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AH15" r:id="rId1"/>
-    <hyperlink ref="AH16:AH19" r:id="rId2" display="\\"/>
+    <hyperlink ref="AH15" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="AH16:AH19" r:id="rId2" display="\\" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B5:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E5">
         <v>0</v>
       </c>
@@ -3469,7 +4336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -3543,7 +4410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>37</v>
       </c>
@@ -3611,7 +4478,7 @@
         <v>0.99981399999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>33</v>
       </c>
@@ -3682,7 +4549,7 @@
         <v>0.99883</v>
       </c>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>37</v>
       </c>
@@ -3750,7 +4617,7 @@
         <v>0.99780599999999997</v>
       </c>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>34</v>
       </c>
@@ -3821,7 +4688,7 @@
         <v>0.91461999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>37</v>
       </c>
@@ -3889,7 +4756,7 @@
         <v>0.87489499999999998</v>
       </c>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>31</v>
       </c>
@@ -3963,7 +4830,7 @@
         <v>0.99982000000000004</v>
       </c>
     </row>
-    <row r="17" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>37</v>
       </c>
@@ -4031,7 +4898,7 @@
         <v>0.99981399999999998</v>
       </c>
     </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>33</v>
       </c>
@@ -4102,7 +4969,7 @@
         <v>0.98748000000000002</v>
       </c>
     </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>37</v>
       </c>
@@ -4170,7 +5037,7 @@
         <v>0.98760599999999998</v>
       </c>
     </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>34</v>
       </c>
@@ -4241,7 +5108,7 @@
         <v>0.87458000000000002</v>
       </c>
     </row>
-    <row r="21" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>37</v>
       </c>
@@ -4314,17 +5181,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -4332,7 +5199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -4340,7 +5207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.2</v>
       </c>
@@ -4348,7 +5215,7 @@
         <v>9.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.3</v>
       </c>
@@ -4356,7 +5223,7 @@
         <v>1.7799999999999999E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.4</v>
       </c>
@@ -4364,7 +5231,7 @@
         <v>1.0690000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -4372,7 +5239,7 @@
         <v>4.2820000000000002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -4380,7 +5247,7 @@
         <v>1.2016000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.7</v>
       </c>
@@ -4388,7 +5255,7 @@
         <v>2.6866000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.8</v>
       </c>
@@ -4396,7 +5263,7 @@
         <v>5.1728000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -4404,7 +5271,7 @@
         <v>8.8322999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4412,7 +5279,7 @@
         <v>0.13741200000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.1000000000000001</v>
       </c>
@@ -4420,7 +5287,7 @@
         <v>0.19964999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.2</v>
       </c>
@@ -4428,7 +5295,7 @@
         <v>0.27320499999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.3</v>
       </c>
@@ -4436,7 +5303,7 @@
         <v>0.35660799999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.4</v>
       </c>
@@ -4444,7 +5311,7 @@
         <v>0.44647999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.5</v>
       </c>
@@ -4452,7 +5319,7 @@
         <v>0.539852</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.6</v>
       </c>
@@ -4460,7 +5327,7 @@
         <v>0.63233099999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.7</v>
       </c>
@@ -4468,7 +5335,7 @@
         <v>0.72029399999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.8</v>
       </c>
@@ -4476,7 +5343,7 @@
         <v>0.79883700000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.9</v>
       </c>
@@ -4484,7 +5351,7 @@
         <v>0.86436400000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
edit price and have result from Server
</commit_message>
<xml_diff>
--- a/K-RRT/excel/setting_KRRT.xlsx
+++ b/K-RRT/excel/setting_KRRT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IDBR\IRDBR\K-RRT\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32EEFDE-894E-4DF4-B7F0-BC8ABA5E4A87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D581CF70-56A5-4D0C-8DD9-F9B9406A4D5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,15 +417,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_noprice" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_price" connectionId="4" xr16:uid="{00000000-0016-0000-0100-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_noprice_1" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="result_noprice" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -698,7 +698,7 @@
   <dimension ref="B3:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12:N16"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
         <v>40</v>
       </c>
       <c r="J12">
-        <v>0.02</v>
+        <v>0.41</v>
       </c>
       <c r="K12">
         <v>500</v>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="M12">
         <f t="shared" ref="M12:M13" si="10">L12*J12</f>
-        <v>61.44</v>
+        <v>1259.52</v>
       </c>
       <c r="N12">
         <f>(L12*8)/(H12+I12)</f>
@@ -1119,7 +1119,7 @@
         <v>50</v>
       </c>
       <c r="J13">
-        <v>0.05</v>
+        <v>0.22</v>
       </c>
       <c r="K13">
         <v>500</v>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="M13">
         <f t="shared" si="10"/>
-        <v>153.60000000000002</v>
+        <v>675.84</v>
       </c>
       <c r="N13">
         <f t="shared" ref="N13:N17" si="11">(L13*8)/(H13+I13)</f>
@@ -1171,7 +1171,7 @@
         <v>60</v>
       </c>
       <c r="J14">
-        <v>0.01</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K14">
         <v>500</v>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="M14">
         <f>L14*J14</f>
-        <v>30.72</v>
+        <v>430.08000000000004</v>
       </c>
       <c r="N14">
         <f t="shared" si="11"/>
@@ -1223,7 +1223,7 @@
         <v>40</v>
       </c>
       <c r="J15">
-        <v>0.02</v>
+        <v>0.25</v>
       </c>
       <c r="K15">
         <v>500</v>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="M15">
         <f t="shared" ref="M15:M17" si="15">L15*J15</f>
-        <v>61.44</v>
+        <v>768</v>
       </c>
       <c r="N15">
         <f t="shared" si="11"/>
@@ -1275,7 +1275,7 @@
         <v>60</v>
       </c>
       <c r="J16">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
       <c r="K16">
         <v>500</v>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="15"/>
-        <v>30.72</v>
+        <v>337.92</v>
       </c>
       <c r="N16">
         <f t="shared" si="11"/>
@@ -1351,7 +1351,7 @@
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="M18">
         <f>AVERAGE(M12:M16)</f>
-        <v>67.584000000000017</v>
+        <v>694.27200000000005</v>
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
   <dimension ref="B3:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>